<commit_message>
updated a whole bunch of shit
dfdfd
</commit_message>
<xml_diff>
--- a/V1/Gui/Sensitivity-0001.xlsx
+++ b/V1/Gui/Sensitivity-0001.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -384,7 +384,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,7 +440,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -448,7 +448,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -456,7 +456,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -464,7 +464,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -472,7 +472,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -480,7 +480,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -488,7 +488,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -496,7 +496,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>